<commit_message>
updated data_formatting and created a short_data sheet in the excel file
</commit_message>
<xml_diff>
--- a/example_data.xlsx
+++ b/example_data.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Koos Oude Lenovo\Google Drive\R manual\R-Manual\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{900AEA33-CAD2-48D1-A999-71C2BBCED689}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F8E01C1-DD65-450D-9F18-56F8A09AEBC7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{123D8167-A480-4849-AFED-0F46F88139D6}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" activeTab="1" xr2:uid="{123D8167-A480-4849-AFED-0F46F88139D6}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
+    <sheet name="short" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="17">
   <si>
     <t>observation</t>
   </si>
@@ -79,6 +80,12 @@
   </si>
   <si>
     <t>day</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>treatment</t>
   </si>
 </sst>
 </file>
@@ -433,7 +440,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33921067-02BE-402D-AAFD-0BF3762ED2DC}">
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
@@ -891,4 +898,75 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A99B5259-C900-4155-A634-5BCADFE4CFE4}">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2">
+        <v>23.6</v>
+      </c>
+      <c r="D2">
+        <v>21.3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3">
+        <v>19.3</v>
+      </c>
+      <c r="D3">
+        <v>17.899999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4">
+        <v>25.8</v>
+      </c>
+      <c r="D4">
+        <v>24.1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>